<commit_message>
with a different learning rate
</commit_message>
<xml_diff>
--- a/res_averages.xlsx
+++ b/res_averages.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="-5600" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="25600" yWindow="-5600" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Pacman Test" sheetId="1" r:id="rId1"/>
@@ -99,8 +99,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -134,7 +136,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -149,6 +151,7 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -163,6 +166,7 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -494,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N138"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101:I101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -525,7 +529,7 @@
         <v>3</v>
       </c>
       <c r="G1">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
@@ -557,7 +561,7 @@
         <v>3</v>
       </c>
       <c r="G2">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="H2" t="s">
         <v>4</v>
@@ -567,7 +571,7 @@
       </c>
       <c r="K2">
         <f>AVERAGE($G$1:G2)</f>
-        <v>8.5</v>
+        <v>13</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>6</v>
@@ -593,17 +597,17 @@
         <v>3</v>
       </c>
       <c r="G3">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="H3" t="s">
         <v>4</v>
       </c>
       <c r="I3">
-        <v>683</v>
+        <v>1000</v>
       </c>
       <c r="K3">
         <f>AVERAGE($G$1:G3)</f>
-        <v>8.3333333333333339</v>
+        <v>13.666666666666666</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -626,7 +630,7 @@
         <v>3</v>
       </c>
       <c r="G4">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H4" t="s">
         <v>4</v>
@@ -636,7 +640,7 @@
       </c>
       <c r="K4">
         <f>AVERAGE($G$1:G4)</f>
-        <v>10.25</v>
+        <v>15.25</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -659,7 +663,7 @@
         <v>3</v>
       </c>
       <c r="G5">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="H5" t="s">
         <v>4</v>
@@ -669,7 +673,7 @@
       </c>
       <c r="K5">
         <f>AVERAGE($G$1:G5)</f>
-        <v>12.2</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -692,17 +696,17 @@
         <v>3</v>
       </c>
       <c r="G6">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="H6" t="s">
         <v>4</v>
       </c>
       <c r="I6">
-        <v>287</v>
+        <v>1000</v>
       </c>
       <c r="K6">
         <f>AVERAGE($G$1:G6)</f>
-        <v>11.333333333333334</v>
+        <v>17.333333333333332</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -725,7 +729,7 @@
         <v>3</v>
       </c>
       <c r="G7">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H7" t="s">
         <v>4</v>
@@ -735,7 +739,7 @@
       </c>
       <c r="K7">
         <f>AVERAGE($G$1:G7)</f>
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -758,7 +762,7 @@
         <v>3</v>
       </c>
       <c r="G8">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="H8" t="s">
         <v>4</v>
@@ -768,7 +772,7 @@
       </c>
       <c r="K8">
         <f>AVERAGE($G$1:G8)</f>
-        <v>13.25</v>
+        <v>16.75</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -791,17 +795,17 @@
         <v>3</v>
       </c>
       <c r="G9">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="H9" t="s">
         <v>4</v>
       </c>
       <c r="I9">
-        <v>1000</v>
+        <v>200</v>
       </c>
       <c r="K9">
         <f>AVERAGE($G$1:G9)</f>
-        <v>13.888888888888889</v>
+        <v>15.555555555555555</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -824,7 +828,7 @@
         <v>3</v>
       </c>
       <c r="G10">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H10" t="s">
         <v>4</v>
@@ -834,7 +838,7 @@
       </c>
       <c r="K10">
         <f>AVERAGE($G$1:G10)</f>
-        <v>13.5</v>
+        <v>14.8</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -857,7 +861,7 @@
         <v>3</v>
       </c>
       <c r="G11">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H11" t="s">
         <v>4</v>
@@ -867,7 +871,7 @@
       </c>
       <c r="K11">
         <f>AVERAGE($G$1:G11)</f>
-        <v>14.090909090909092</v>
+        <v>15.363636363636363</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -890,7 +894,7 @@
         <v>3</v>
       </c>
       <c r="G12">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="H12" t="s">
         <v>4</v>
@@ -900,7 +904,7 @@
       </c>
       <c r="K12">
         <f>AVERAGE($G$1:G12)</f>
-        <v>14.166666666666666</v>
+        <v>14.75</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -923,17 +927,17 @@
         <v>3</v>
       </c>
       <c r="G13">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="H13" t="s">
         <v>4</v>
       </c>
       <c r="I13">
-        <v>593</v>
+        <v>1000</v>
       </c>
       <c r="K13">
         <f>AVERAGE($G$1:G13)</f>
-        <v>13.76923076923077</v>
+        <v>15.076923076923077</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -956,7 +960,7 @@
         <v>3</v>
       </c>
       <c r="G14">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H14" t="s">
         <v>4</v>
@@ -966,7 +970,7 @@
       </c>
       <c r="K14">
         <f>AVERAGE($G$1:G14)</f>
-        <v>14.071428571428571</v>
+        <v>15.071428571428571</v>
       </c>
     </row>
     <row r="15" spans="1:14">
@@ -989,17 +993,17 @@
         <v>3</v>
       </c>
       <c r="G15">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="H15" t="s">
         <v>4</v>
       </c>
       <c r="I15">
-        <v>209</v>
+        <v>1000</v>
       </c>
       <c r="K15">
         <f>AVERAGE($G$1:G15)</f>
-        <v>13.6</v>
+        <v>15.6</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -1022,7 +1026,7 @@
         <v>3</v>
       </c>
       <c r="G16">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H16" t="s">
         <v>4</v>
@@ -1032,7 +1036,7 @@
       </c>
       <c r="K16">
         <f>AVERAGE($G$1:G16)</f>
-        <v>14.4375</v>
+        <v>15.9375</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1055,7 +1059,7 @@
         <v>3</v>
       </c>
       <c r="G17">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="H17" t="s">
         <v>4</v>
@@ -1065,7 +1069,7 @@
       </c>
       <c r="K17">
         <f>AVERAGE($G$1:G17)</f>
-        <v>14.529411764705882</v>
+        <v>16.941176470588236</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1088,7 +1092,7 @@
         <v>3</v>
       </c>
       <c r="G18">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="H18" t="s">
         <v>4</v>
@@ -1098,7 +1102,7 @@
       </c>
       <c r="K18">
         <f>AVERAGE($G$1:G18)</f>
-        <v>15</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1121,17 +1125,17 @@
         <v>3</v>
       </c>
       <c r="G19">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H19" t="s">
         <v>4</v>
       </c>
       <c r="I19">
-        <v>341</v>
+        <v>1000</v>
       </c>
       <c r="K19">
         <f>AVERAGE($G$1:G19)</f>
-        <v>15.052631578947368</v>
+        <v>17.631578947368421</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1154,17 +1158,17 @@
         <v>3</v>
       </c>
       <c r="G20">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="H20" t="s">
         <v>4</v>
       </c>
       <c r="I20">
-        <v>509</v>
+        <v>1000</v>
       </c>
       <c r="K20">
         <f>AVERAGE($G$1:G20)</f>
-        <v>14.65</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1187,7 +1191,7 @@
         <v>3</v>
       </c>
       <c r="G21">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="H21" t="s">
         <v>4</v>
@@ -1197,7 +1201,7 @@
       </c>
       <c r="K21">
         <f>AVERAGE($G$1:G21)</f>
-        <v>14.761904761904763</v>
+        <v>17.904761904761905</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1220,7 +1224,7 @@
         <v>3</v>
       </c>
       <c r="G22">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="H22" t="s">
         <v>4</v>
@@ -1230,7 +1234,7 @@
       </c>
       <c r="K22">
         <f>AVERAGE($G$1:G22)</f>
-        <v>15.272727272727273</v>
+        <v>17.772727272727273</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1253,7 +1257,7 @@
         <v>3</v>
       </c>
       <c r="G23">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="H23" t="s">
         <v>4</v>
@@ -1263,7 +1267,7 @@
       </c>
       <c r="K23">
         <f>AVERAGE($G$1:G23)</f>
-        <v>14.956521739130435</v>
+        <v>18.130434782608695</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1286,7 +1290,7 @@
         <v>3</v>
       </c>
       <c r="G24">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="H24" t="s">
         <v>4</v>
@@ -1296,7 +1300,7 @@
       </c>
       <c r="K24">
         <f>AVERAGE($G$1:G24)</f>
-        <v>14.833333333333334</v>
+        <v>18.083333333333332</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1319,7 +1323,7 @@
         <v>3</v>
       </c>
       <c r="G25">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="H25" t="s">
         <v>4</v>
@@ -1329,7 +1333,7 @@
       </c>
       <c r="K25">
         <f>AVERAGE($G$1:G25)</f>
-        <v>15.16</v>
+        <v>17.84</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1352,7 +1356,7 @@
         <v>3</v>
       </c>
       <c r="G26">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H26" t="s">
         <v>4</v>
@@ -1362,7 +1366,7 @@
       </c>
       <c r="K26">
         <f>AVERAGE($G$1:G26)</f>
-        <v>15.307692307692308</v>
+        <v>17.846153846153847</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1385,7 +1389,7 @@
         <v>3</v>
       </c>
       <c r="G27">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H27" t="s">
         <v>4</v>
@@ -1395,7 +1399,7 @@
       </c>
       <c r="K27">
         <f>AVERAGE($G$1:G27)</f>
-        <v>15.481481481481481</v>
+        <v>18.111111111111111</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1418,7 +1422,7 @@
         <v>3</v>
       </c>
       <c r="G28">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="H28" t="s">
         <v>4</v>
@@ -1428,7 +1432,7 @@
       </c>
       <c r="K28">
         <f>AVERAGE($G$1:G28)</f>
-        <v>15.607142857142858</v>
+        <v>17.714285714285715</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1451,7 +1455,7 @@
         <v>3</v>
       </c>
       <c r="G29">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H29" t="s">
         <v>4</v>
@@ -1461,7 +1465,7 @@
       </c>
       <c r="K29">
         <f>AVERAGE($G$1:G29)</f>
-        <v>15.827586206896552</v>
+        <v>17.758620689655171</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1484,7 +1488,7 @@
         <v>3</v>
       </c>
       <c r="G30">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="H30" t="s">
         <v>4</v>
@@ -1494,7 +1498,7 @@
       </c>
       <c r="K30">
         <f>AVERAGE($G$1:G30)</f>
-        <v>15.7</v>
+        <v>18.133333333333333</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1517,17 +1521,17 @@
         <v>3</v>
       </c>
       <c r="G31">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="H31" t="s">
         <v>4</v>
       </c>
       <c r="I31">
-        <v>203</v>
+        <v>1000</v>
       </c>
       <c r="K31">
         <f>AVERAGE($G$1:G31)</f>
-        <v>15.387096774193548</v>
+        <v>18.161290322580644</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -1550,7 +1554,7 @@
         <v>3</v>
       </c>
       <c r="G32">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="H32" t="s">
         <v>4</v>
@@ -1560,7 +1564,7 @@
       </c>
       <c r="K32">
         <f>AVERAGE($G$1:G32)</f>
-        <v>15.53125</v>
+        <v>18.34375</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -1583,17 +1587,17 @@
         <v>3</v>
       </c>
       <c r="G33">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="H33" t="s">
         <v>4</v>
       </c>
       <c r="I33">
-        <v>371</v>
+        <v>1000</v>
       </c>
       <c r="K33">
         <f>AVERAGE($G$1:G33)</f>
-        <v>15.363636363636363</v>
+        <v>18.363636363636363</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -1616,17 +1620,17 @@
         <v>3</v>
       </c>
       <c r="G34">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="H34" t="s">
         <v>4</v>
       </c>
       <c r="I34">
-        <v>503</v>
+        <v>1000</v>
       </c>
       <c r="K34">
         <f>AVERAGE($G$1:G34)</f>
-        <v>16.088235294117649</v>
+        <v>18.264705882352942</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -1659,7 +1663,7 @@
       </c>
       <c r="K35">
         <f>AVERAGE($G$1:G35)</f>
-        <v>16.228571428571428</v>
+        <v>18.342857142857142</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -1682,7 +1686,7 @@
         <v>3</v>
       </c>
       <c r="G36">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H36" t="s">
         <v>4</v>
@@ -1692,7 +1696,7 @@
       </c>
       <c r="K36">
         <f>AVERAGE($G$1:G36)</f>
-        <v>16.305555555555557</v>
+        <v>18.527777777777779</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -1715,17 +1719,17 @@
         <v>3</v>
       </c>
       <c r="G37">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="H37" t="s">
         <v>4</v>
       </c>
       <c r="I37">
-        <v>611</v>
+        <v>1000</v>
       </c>
       <c r="K37">
         <f>AVERAGE($G$1:G37)</f>
-        <v>16.378378378378379</v>
+        <v>18.972972972972972</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -1748,17 +1752,17 @@
         <v>3</v>
       </c>
       <c r="G38">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="H38" t="s">
         <v>4</v>
       </c>
       <c r="I38">
-        <v>1000</v>
+        <v>764</v>
       </c>
       <c r="K38">
         <f>AVERAGE($G$1:G38)</f>
-        <v>16.578947368421051</v>
+        <v>18.631578947368421</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -1781,17 +1785,17 @@
         <v>3</v>
       </c>
       <c r="G39">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H39" t="s">
         <v>4</v>
       </c>
       <c r="I39">
-        <v>439</v>
+        <v>1000</v>
       </c>
       <c r="K39">
         <f>AVERAGE($G$1:G39)</f>
-        <v>16.46153846153846</v>
+        <v>18.512820512820515</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -1814,7 +1818,7 @@
         <v>3</v>
       </c>
       <c r="G40">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="H40" t="s">
         <v>4</v>
@@ -1824,7 +1828,7 @@
       </c>
       <c r="K40">
         <f>AVERAGE($G$1:G40)</f>
-        <v>16.425000000000001</v>
+        <v>19.3</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -1847,7 +1851,7 @@
         <v>3</v>
       </c>
       <c r="G41">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="H41" t="s">
         <v>4</v>
@@ -1857,7 +1861,7 @@
       </c>
       <c r="K41">
         <f>AVERAGE($G$1:G41)</f>
-        <v>16.634146341463413</v>
+        <v>19.756097560975611</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -1880,17 +1884,17 @@
         <v>3</v>
       </c>
       <c r="G42">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H42" t="s">
         <v>4</v>
       </c>
       <c r="I42">
-        <v>792</v>
+        <v>1000</v>
       </c>
       <c r="K42">
         <f>AVERAGE($G$1:G42)</f>
-        <v>16.833333333333332</v>
+        <v>19.761904761904763</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -1913,7 +1917,7 @@
         <v>3</v>
       </c>
       <c r="G43">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H43" t="s">
         <v>4</v>
@@ -1923,7 +1927,7 @@
       </c>
       <c r="K43">
         <f>AVERAGE($G$1:G43)</f>
-        <v>16.88372093023256</v>
+        <v>19.790697674418606</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -1946,7 +1950,7 @@
         <v>3</v>
       </c>
       <c r="G44">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="H44" t="s">
         <v>4</v>
@@ -1956,7 +1960,7 @@
       </c>
       <c r="K44">
         <f>AVERAGE($G$1:G44)</f>
-        <v>17.545454545454547</v>
+        <v>19.886363636363637</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -1979,7 +1983,7 @@
         <v>3</v>
       </c>
       <c r="G45">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="H45" t="s">
         <v>4</v>
@@ -1989,7 +1993,7 @@
       </c>
       <c r="K45">
         <f>AVERAGE($G$1:G45)</f>
-        <v>17.555555555555557</v>
+        <v>20.31111111111111</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -2012,17 +2016,17 @@
         <v>3</v>
       </c>
       <c r="G46">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="H46" t="s">
         <v>4</v>
       </c>
       <c r="I46">
-        <v>875</v>
+        <v>1000</v>
       </c>
       <c r="K46">
         <f>AVERAGE($G$1:G46)</f>
-        <v>17.869565217391305</v>
+        <v>20.304347826086957</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -2045,7 +2049,7 @@
         <v>3</v>
       </c>
       <c r="G47">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="H47" t="s">
         <v>4</v>
@@ -2055,7 +2059,7 @@
       </c>
       <c r="K47">
         <f>AVERAGE($G$1:G47)</f>
-        <v>18.148936170212767</v>
+        <v>20.340425531914892</v>
       </c>
     </row>
     <row r="48" spans="1:11">
@@ -2078,17 +2082,17 @@
         <v>3</v>
       </c>
       <c r="G48">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="H48" t="s">
         <v>4</v>
       </c>
       <c r="I48">
-        <v>362</v>
+        <v>1000</v>
       </c>
       <c r="K48">
         <f>AVERAGE($G$1:G48)</f>
-        <v>17.979166666666668</v>
+        <v>20.291666666666668</v>
       </c>
     </row>
     <row r="49" spans="1:11">
@@ -2111,7 +2115,7 @@
         <v>3</v>
       </c>
       <c r="G49">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="H49" t="s">
         <v>4</v>
@@ -2121,7 +2125,7 @@
       </c>
       <c r="K49">
         <f>AVERAGE($G$1:G49)</f>
-        <v>18.346938775510203</v>
+        <v>20.346938775510203</v>
       </c>
     </row>
     <row r="50" spans="1:11">
@@ -2144,7 +2148,7 @@
         <v>3</v>
       </c>
       <c r="G50">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H50" t="s">
         <v>4</v>
@@ -2154,7 +2158,7 @@
       </c>
       <c r="K50">
         <f>AVERAGE($G$1:G50)</f>
-        <v>18.28</v>
+        <v>20.22</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -2177,7 +2181,7 @@
         <v>3</v>
       </c>
       <c r="G51">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="H51" t="s">
         <v>4</v>
@@ -2187,7 +2191,7 @@
       </c>
       <c r="K51">
         <f>AVERAGE($G$1:G51)</f>
-        <v>18.470588235294116</v>
+        <v>20.176470588235293</v>
       </c>
     </row>
     <row r="52" spans="1:11">
@@ -2210,7 +2214,7 @@
         <v>3</v>
       </c>
       <c r="G52">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="H52" t="s">
         <v>4</v>
@@ -2220,7 +2224,7 @@
       </c>
       <c r="K52">
         <f>AVERAGE($G$1:G52)</f>
-        <v>18.826923076923077</v>
+        <v>20.134615384615383</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -2243,7 +2247,7 @@
         <v>3</v>
       </c>
       <c r="G53">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="H53" t="s">
         <v>4</v>
@@ -2253,7 +2257,7 @@
       </c>
       <c r="K53">
         <f>AVERAGE($G$1:G53)</f>
-        <v>18.867924528301888</v>
+        <v>20.30188679245283</v>
       </c>
     </row>
     <row r="54" spans="1:11">
@@ -2276,17 +2280,17 @@
         <v>3</v>
       </c>
       <c r="G54">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="H54" t="s">
         <v>4</v>
       </c>
       <c r="I54">
-        <v>1000</v>
+        <v>512</v>
       </c>
       <c r="K54">
         <f>AVERAGE($G$1:G54)</f>
-        <v>19.092592592592592</v>
+        <v>20.111111111111111</v>
       </c>
     </row>
     <row r="55" spans="1:11">
@@ -2309,7 +2313,7 @@
         <v>3</v>
       </c>
       <c r="G55">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H55" t="s">
         <v>4</v>
@@ -2319,7 +2323,7 @@
       </c>
       <c r="K55">
         <f>AVERAGE($G$1:G55)</f>
-        <v>19.145454545454545</v>
+        <v>20.109090909090909</v>
       </c>
     </row>
     <row r="56" spans="1:11">
@@ -2342,7 +2346,7 @@
         <v>3</v>
       </c>
       <c r="G56">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="H56" t="s">
         <v>4</v>
@@ -2352,7 +2356,7 @@
       </c>
       <c r="K56">
         <f>AVERAGE($G$1:G56)</f>
-        <v>19.178571428571427</v>
+        <v>20.267857142857142</v>
       </c>
     </row>
     <row r="57" spans="1:11">
@@ -2375,7 +2379,7 @@
         <v>3</v>
       </c>
       <c r="G57">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="H57" t="s">
         <v>4</v>
@@ -2385,7 +2389,7 @@
       </c>
       <c r="K57">
         <f>AVERAGE($G$1:G57)</f>
-        <v>19.684210526315791</v>
+        <v>20.263157894736842</v>
       </c>
     </row>
     <row r="58" spans="1:11">
@@ -2408,7 +2412,7 @@
         <v>3</v>
       </c>
       <c r="G58">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="H58" t="s">
         <v>4</v>
@@ -2418,7 +2422,7 @@
       </c>
       <c r="K58">
         <f>AVERAGE($G$1:G58)</f>
-        <v>19.551724137931036</v>
+        <v>20.241379310344829</v>
       </c>
     </row>
     <row r="59" spans="1:11">
@@ -2441,17 +2445,17 @@
         <v>3</v>
       </c>
       <c r="G59">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="H59" t="s">
         <v>4</v>
       </c>
       <c r="I59">
-        <v>1000</v>
+        <v>416</v>
       </c>
       <c r="K59">
         <f>AVERAGE($G$1:G59)</f>
-        <v>19.508474576271187</v>
+        <v>20</v>
       </c>
     </row>
     <row r="60" spans="1:11">
@@ -2474,7 +2478,7 @@
         <v>3</v>
       </c>
       <c r="G60">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H60" t="s">
         <v>4</v>
@@ -2484,7 +2488,7 @@
       </c>
       <c r="K60">
         <f>AVERAGE($G$1:G60)</f>
-        <v>19.516666666666666</v>
+        <v>19.983333333333334</v>
       </c>
     </row>
     <row r="61" spans="1:11">
@@ -2507,17 +2511,17 @@
         <v>3</v>
       </c>
       <c r="G61">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H61" t="s">
         <v>4</v>
       </c>
       <c r="I61">
-        <v>629</v>
+        <v>1000</v>
       </c>
       <c r="K61">
         <f>AVERAGE($G$1:G61)</f>
-        <v>19.606557377049182</v>
+        <v>20</v>
       </c>
     </row>
     <row r="62" spans="1:11">
@@ -2540,17 +2544,17 @@
         <v>3</v>
       </c>
       <c r="G62">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="H62" t="s">
         <v>4</v>
       </c>
       <c r="I62">
-        <v>770</v>
+        <v>1000</v>
       </c>
       <c r="K62">
         <f>AVERAGE($G$1:G62)</f>
-        <v>19.693548387096776</v>
+        <v>19.903225806451612</v>
       </c>
     </row>
     <row r="63" spans="1:11">
@@ -2573,7 +2577,7 @@
         <v>3</v>
       </c>
       <c r="G63">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H63" t="s">
         <v>4</v>
@@ -2583,7 +2587,7 @@
       </c>
       <c r="K63">
         <f>AVERAGE($G$1:G63)</f>
-        <v>19.80952380952381</v>
+        <v>19.936507936507937</v>
       </c>
     </row>
     <row r="64" spans="1:11">
@@ -2606,17 +2610,17 @@
         <v>3</v>
       </c>
       <c r="G64">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H64" t="s">
         <v>4</v>
       </c>
       <c r="I64">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="K64">
         <f>AVERAGE($G$1:G64)</f>
-        <v>19.765625</v>
+        <v>19.828125</v>
       </c>
     </row>
     <row r="65" spans="1:11">
@@ -2639,7 +2643,7 @@
         <v>3</v>
       </c>
       <c r="G65">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="H65" t="s">
         <v>4</v>
@@ -2649,7 +2653,7 @@
       </c>
       <c r="K65">
         <f>AVERAGE($G$1:G65)</f>
-        <v>19.784615384615385</v>
+        <v>20.138461538461538</v>
       </c>
     </row>
     <row r="66" spans="1:11">
@@ -2672,7 +2676,7 @@
         <v>3</v>
       </c>
       <c r="G66">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="H66" t="s">
         <v>4</v>
@@ -2682,7 +2686,7 @@
       </c>
       <c r="K66">
         <f>AVERAGE($G$1:G66)</f>
-        <v>20.166666666666668</v>
+        <v>19.939393939393938</v>
       </c>
     </row>
     <row r="67" spans="1:11">
@@ -2705,7 +2709,7 @@
         <v>3</v>
       </c>
       <c r="G67">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="H67" t="s">
         <v>4</v>
@@ -2715,7 +2719,7 @@
       </c>
       <c r="K67">
         <f>AVERAGE($G$1:G67)</f>
-        <v>20.149253731343283</v>
+        <v>19.791044776119403</v>
       </c>
     </row>
     <row r="68" spans="1:11">
@@ -2738,17 +2742,17 @@
         <v>3</v>
       </c>
       <c r="G68">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="H68" t="s">
         <v>4</v>
       </c>
       <c r="I68">
-        <v>365</v>
+        <v>1000</v>
       </c>
       <c r="K68">
         <f>AVERAGE($G$1:G68)</f>
-        <v>19.955882352941178</v>
+        <v>19.867647058823529</v>
       </c>
     </row>
     <row r="69" spans="1:11">
@@ -2771,7 +2775,7 @@
         <v>3</v>
       </c>
       <c r="G69">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H69" t="s">
         <v>4</v>
@@ -2781,7 +2785,7 @@
       </c>
       <c r="K69">
         <f>AVERAGE($G$1:G69)</f>
-        <v>20.057971014492754</v>
+        <v>19.927536231884059</v>
       </c>
     </row>
     <row r="70" spans="1:11">
@@ -2804,17 +2808,17 @@
         <v>3</v>
       </c>
       <c r="G70">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="H70" t="s">
         <v>4</v>
       </c>
       <c r="I70">
-        <v>506</v>
+        <v>448</v>
       </c>
       <c r="K70">
         <f>AVERAGE($G$1:G70)</f>
-        <v>20.042857142857144</v>
+        <v>19.728571428571428</v>
       </c>
     </row>
     <row r="71" spans="1:11">
@@ -2837,7 +2841,7 @@
         <v>3</v>
       </c>
       <c r="G71">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="H71" t="s">
         <v>4</v>
@@ -2847,7 +2851,7 @@
       </c>
       <c r="K71">
         <f>AVERAGE($G$1:G71)</f>
-        <v>20.04225352112676</v>
+        <v>19.676056338028168</v>
       </c>
     </row>
     <row r="72" spans="1:11">
@@ -2870,7 +2874,7 @@
         <v>3</v>
       </c>
       <c r="G72">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="H72" t="s">
         <v>4</v>
@@ -2880,7 +2884,7 @@
       </c>
       <c r="K72">
         <f>AVERAGE($G$1:G72)</f>
-        <v>20.097222222222221</v>
+        <v>19.583333333333332</v>
       </c>
     </row>
     <row r="73" spans="1:11">
@@ -2903,7 +2907,7 @@
         <v>3</v>
       </c>
       <c r="G73">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="H73" t="s">
         <v>4</v>
@@ -2913,7 +2917,7 @@
       </c>
       <c r="K73">
         <f>AVERAGE($G$1:G73)</f>
-        <v>20.123287671232877</v>
+        <v>19.698630136986303</v>
       </c>
     </row>
     <row r="74" spans="1:11">
@@ -2936,7 +2940,7 @@
         <v>3</v>
       </c>
       <c r="G74">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H74" t="s">
         <v>4</v>
@@ -2946,7 +2950,7 @@
       </c>
       <c r="K74">
         <f>AVERAGE($G$1:G74)</f>
-        <v>20.216216216216218</v>
+        <v>19.716216216216218</v>
       </c>
     </row>
     <row r="75" spans="1:11">
@@ -2969,17 +2973,17 @@
         <v>3</v>
       </c>
       <c r="G75">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="H75" t="s">
         <v>4</v>
       </c>
       <c r="I75">
-        <v>722</v>
+        <v>203</v>
       </c>
       <c r="K75">
         <f>AVERAGE($G$1:G75)</f>
-        <v>20.239999999999998</v>
+        <v>19.533333333333335</v>
       </c>
     </row>
     <row r="76" spans="1:11">
@@ -3002,7 +3006,7 @@
         <v>3</v>
       </c>
       <c r="G76">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H76" t="s">
         <v>4</v>
@@ -3012,7 +3016,7 @@
       </c>
       <c r="K76">
         <f>AVERAGE($G$1:G76)</f>
-        <v>20.25</v>
+        <v>19.526315789473685</v>
       </c>
     </row>
     <row r="77" spans="1:11">
@@ -3035,7 +3039,7 @@
         <v>3</v>
       </c>
       <c r="G77">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="H77" t="s">
         <v>4</v>
@@ -3045,7 +3049,7 @@
       </c>
       <c r="K77">
         <f>AVERAGE($G$1:G77)</f>
-        <v>20.61038961038961</v>
+        <v>19.532467532467532</v>
       </c>
     </row>
     <row r="78" spans="1:11">
@@ -3068,7 +3072,7 @@
         <v>3</v>
       </c>
       <c r="G78">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="H78" t="s">
         <v>4</v>
@@ -3078,7 +3082,7 @@
       </c>
       <c r="K78">
         <f>AVERAGE($G$1:G78)</f>
-        <v>20.615384615384617</v>
+        <v>19.487179487179485</v>
       </c>
     </row>
     <row r="79" spans="1:11">
@@ -3101,17 +3105,17 @@
         <v>3</v>
       </c>
       <c r="G79">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="H79" t="s">
         <v>4</v>
       </c>
       <c r="I79">
-        <v>1000</v>
+        <v>198</v>
       </c>
       <c r="K79">
         <f>AVERAGE($G$1:G79)</f>
-        <v>20.594936708860761</v>
+        <v>19.316455696202532</v>
       </c>
     </row>
     <row r="80" spans="1:11">
@@ -3134,7 +3138,7 @@
         <v>3</v>
       </c>
       <c r="G80">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H80" t="s">
         <v>4</v>
@@ -3144,7 +3148,7 @@
       </c>
       <c r="K80">
         <f>AVERAGE($G$1:G80)</f>
-        <v>20.625</v>
+        <v>19.375</v>
       </c>
     </row>
     <row r="81" spans="1:11">
@@ -3167,7 +3171,7 @@
         <v>3</v>
       </c>
       <c r="G81">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="H81" t="s">
         <v>4</v>
@@ -3177,7 +3181,7 @@
       </c>
       <c r="K81">
         <f>AVERAGE($G$1:G81)</f>
-        <v>20.790123456790123</v>
+        <v>19.308641975308642</v>
       </c>
     </row>
     <row r="82" spans="1:11">
@@ -3200,7 +3204,7 @@
         <v>3</v>
       </c>
       <c r="G82">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="H82" t="s">
         <v>4</v>
@@ -3210,7 +3214,7 @@
       </c>
       <c r="K82">
         <f>AVERAGE($G$1:G82)</f>
-        <v>20.865853658536587</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="83" spans="1:11">
@@ -3233,17 +3237,17 @@
         <v>3</v>
       </c>
       <c r="G83">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="H83" t="s">
         <v>4</v>
       </c>
       <c r="I83">
-        <v>440</v>
+        <v>1000</v>
       </c>
       <c r="K83">
         <f>AVERAGE($G$1:G83)</f>
-        <v>21.024096385542169</v>
+        <v>19.518072289156628</v>
       </c>
     </row>
     <row r="84" spans="1:11">
@@ -3266,17 +3270,17 @@
         <v>3</v>
       </c>
       <c r="G84">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H84" t="s">
         <v>4</v>
       </c>
       <c r="I84">
-        <v>1000</v>
+        <v>671</v>
       </c>
       <c r="K84">
         <f>AVERAGE($G$1:G84)</f>
-        <v>21</v>
+        <v>19.488095238095237</v>
       </c>
     </row>
     <row r="85" spans="1:11">
@@ -3299,7 +3303,7 @@
         <v>3</v>
       </c>
       <c r="G85">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="H85" t="s">
         <v>4</v>
@@ -3309,7 +3313,7 @@
       </c>
       <c r="K85">
         <f>AVERAGE($G$1:G85)</f>
-        <v>21.129411764705882</v>
+        <v>19.423529411764704</v>
       </c>
     </row>
     <row r="86" spans="1:11">
@@ -3332,17 +3336,17 @@
         <v>3</v>
       </c>
       <c r="G86">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H86" t="s">
         <v>4</v>
       </c>
       <c r="I86">
-        <v>434</v>
+        <v>1000</v>
       </c>
       <c r="K86">
         <f>AVERAGE($G$1:G86)</f>
-        <v>21.209302325581394</v>
+        <v>19.534883720930232</v>
       </c>
     </row>
     <row r="87" spans="1:11">
@@ -3365,17 +3369,17 @@
         <v>3</v>
       </c>
       <c r="G87">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="H87" t="s">
         <v>4</v>
       </c>
       <c r="I87">
-        <v>737</v>
+        <v>1000</v>
       </c>
       <c r="K87">
         <f>AVERAGE($G$1:G87)</f>
-        <v>21.045977011494251</v>
+        <v>19.505747126436781</v>
       </c>
     </row>
     <row r="88" spans="1:11">
@@ -3398,17 +3402,17 @@
         <v>3</v>
       </c>
       <c r="G88">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H88" t="s">
         <v>4</v>
       </c>
       <c r="I88">
-        <v>472</v>
+        <v>371</v>
       </c>
       <c r="K88">
         <f>AVERAGE($G$1:G88)</f>
-        <v>21</v>
+        <v>19.420454545454547</v>
       </c>
     </row>
     <row r="89" spans="1:11">
@@ -3431,7 +3435,7 @@
         <v>3</v>
       </c>
       <c r="G89">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H89" t="s">
         <v>4</v>
@@ -3441,7 +3445,7 @@
       </c>
       <c r="K89">
         <f>AVERAGE($G$1:G89)</f>
-        <v>20.910112359550563</v>
+        <v>19.337078651685392</v>
       </c>
     </row>
     <row r="90" spans="1:11">
@@ -3464,7 +3468,7 @@
         <v>3</v>
       </c>
       <c r="G90">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="H90" t="s">
         <v>4</v>
@@ -3474,7 +3478,7 @@
       </c>
       <c r="K90">
         <f>AVERAGE($G$1:G90)</f>
-        <v>21.177777777777777</v>
+        <v>19.211111111111112</v>
       </c>
     </row>
     <row r="91" spans="1:11">
@@ -3497,7 +3501,7 @@
         <v>3</v>
       </c>
       <c r="G91">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="H91" t="s">
         <v>4</v>
@@ -3507,7 +3511,7 @@
       </c>
       <c r="K91">
         <f>AVERAGE($G$1:G91)</f>
-        <v>21.53846153846154</v>
+        <v>19.340659340659339</v>
       </c>
     </row>
     <row r="92" spans="1:11">
@@ -3530,7 +3534,7 @@
         <v>3</v>
       </c>
       <c r="G92">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H92" t="s">
         <v>4</v>
@@ -3540,7 +3544,7 @@
       </c>
       <c r="K92">
         <f>AVERAGE($G$1:G92)</f>
-        <v>21.5</v>
+        <v>19.282608695652176</v>
       </c>
     </row>
     <row r="93" spans="1:11">
@@ -3563,7 +3567,7 @@
         <v>3</v>
       </c>
       <c r="G93">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H93" t="s">
         <v>4</v>
@@ -3573,7 +3577,7 @@
       </c>
       <c r="K93">
         <f>AVERAGE($G$1:G93)</f>
-        <v>21.537634408602152</v>
+        <v>19.29032258064516</v>
       </c>
     </row>
     <row r="94" spans="1:11">
@@ -3596,17 +3600,17 @@
         <v>3</v>
       </c>
       <c r="G94">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H94" t="s">
         <v>4</v>
       </c>
       <c r="I94">
-        <v>253</v>
+        <v>500</v>
       </c>
       <c r="K94">
         <f>AVERAGE($G$1:G94)</f>
-        <v>21.372340425531913</v>
+        <v>19.159574468085108</v>
       </c>
     </row>
     <row r="95" spans="1:11">
@@ -3629,17 +3633,17 @@
         <v>3</v>
       </c>
       <c r="G95">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="H95" t="s">
         <v>4</v>
       </c>
       <c r="I95">
-        <v>419</v>
+        <v>1000</v>
       </c>
       <c r="K95">
         <f>AVERAGE($G$1:G95)</f>
-        <v>21.221052631578946</v>
+        <v>19.094736842105263</v>
       </c>
     </row>
     <row r="96" spans="1:11">
@@ -3662,7 +3666,7 @@
         <v>3</v>
       </c>
       <c r="G96">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="H96" t="s">
         <v>4</v>
@@ -3672,7 +3676,7 @@
       </c>
       <c r="K96">
         <f>AVERAGE($G$1:G96)</f>
-        <v>21.1875</v>
+        <v>19.15625</v>
       </c>
     </row>
     <row r="97" spans="1:11">
@@ -3695,17 +3699,17 @@
         <v>3</v>
       </c>
       <c r="G97">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="H97" t="s">
         <v>4</v>
       </c>
       <c r="I97">
-        <v>302</v>
+        <v>1000</v>
       </c>
       <c r="K97">
         <f>AVERAGE($G$1:G97)</f>
-        <v>21.030927835051546</v>
+        <v>19.422680412371133</v>
       </c>
     </row>
     <row r="98" spans="1:11">
@@ -3728,7 +3732,7 @@
         <v>3</v>
       </c>
       <c r="G98">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H98" t="s">
         <v>4</v>
@@ -3738,7 +3742,7 @@
       </c>
       <c r="K98">
         <f>AVERAGE($G$1:G98)</f>
-        <v>21.020408163265305</v>
+        <v>19.377551020408163</v>
       </c>
     </row>
     <row r="99" spans="1:11">
@@ -3761,7 +3765,7 @@
         <v>3</v>
       </c>
       <c r="G99">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H99" t="s">
         <v>4</v>
@@ -3771,7 +3775,7 @@
       </c>
       <c r="K99">
         <f>AVERAGE($G$1:G99)</f>
-        <v>21.040404040404042</v>
+        <v>19.393939393939394</v>
       </c>
     </row>
     <row r="100" spans="1:11">
@@ -3794,17 +3798,17 @@
         <v>3</v>
       </c>
       <c r="G100">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="H100" t="s">
         <v>4</v>
       </c>
       <c r="I100">
-        <v>371</v>
+        <v>1000</v>
       </c>
       <c r="K100">
         <f>AVERAGE($G$1:G100)</f>
-        <v>20.93</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="101" spans="1:11">
@@ -3824,7 +3828,7 @@
         <v>3</v>
       </c>
       <c r="G101">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="H101" t="s">
         <v>4</v>
@@ -3834,229 +3838,229 @@
       </c>
       <c r="K101">
         <f>AVERAGE($G$1:G101)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="102" spans="1:11">
       <c r="K102">
         <f>AVERAGE($G$1:G102)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="103" spans="1:11">
       <c r="K103">
         <f>AVERAGE($G$1:G103)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="104" spans="1:11">
       <c r="K104">
         <f>AVERAGE($G$1:G104)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="105" spans="1:11">
       <c r="K105">
         <f>AVERAGE($G$1:G105)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="106" spans="1:11">
       <c r="K106">
         <f>AVERAGE($G$1:G106)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="107" spans="1:11">
       <c r="K107">
         <f>AVERAGE($G$1:G107)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="108" spans="1:11">
       <c r="K108">
         <f>AVERAGE($G$1:G108)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="109" spans="1:11">
       <c r="K109">
         <f>AVERAGE($G$1:G109)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="110" spans="1:11">
       <c r="K110">
         <f>AVERAGE($G$1:G110)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="111" spans="1:11">
       <c r="K111">
         <f>AVERAGE($G$1:G111)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="112" spans="1:11">
       <c r="K112">
         <f>AVERAGE($G$1:G112)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="113" spans="11:11">
       <c r="K113">
         <f>AVERAGE($G$1:G113)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="114" spans="11:11">
       <c r="K114">
         <f>AVERAGE($G$1:G114)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="115" spans="11:11">
       <c r="K115">
         <f>AVERAGE($G$1:G115)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="116" spans="11:11">
       <c r="K116">
         <f>AVERAGE($G$1:G116)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="117" spans="11:11">
       <c r="K117">
         <f>AVERAGE($G$1:G117)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="118" spans="11:11">
       <c r="K118">
         <f>AVERAGE($G$1:G118)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="119" spans="11:11">
       <c r="K119">
         <f>AVERAGE($G$1:G119)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="120" spans="11:11">
       <c r="K120">
         <f>AVERAGE($G$1:G120)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="121" spans="11:11">
       <c r="K121">
         <f>AVERAGE($G$1:G121)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="122" spans="11:11">
       <c r="K122">
         <f>AVERAGE($G$1:G122)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="123" spans="11:11">
       <c r="K123">
         <f>AVERAGE($G$1:G123)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="124" spans="11:11">
       <c r="K124">
         <f>AVERAGE($G$1:G124)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="125" spans="11:11">
       <c r="K125">
         <f>AVERAGE($G$1:G125)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="126" spans="11:11">
       <c r="K126">
         <f>AVERAGE($G$1:G126)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="127" spans="11:11">
       <c r="K127">
         <f>AVERAGE($G$1:G127)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="128" spans="11:11">
       <c r="K128">
         <f>AVERAGE($G$1:G128)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="129" spans="11:11">
       <c r="K129">
         <f>AVERAGE($G$1:G129)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="130" spans="11:11">
       <c r="K130">
         <f>AVERAGE($G$1:G130)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="131" spans="11:11">
       <c r="K131">
         <f>AVERAGE($G$1:G131)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="132" spans="11:11">
       <c r="K132">
         <f>AVERAGE($G$1:G132)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="133" spans="11:11">
       <c r="K133">
         <f>AVERAGE($G$1:G133)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="134" spans="11:11">
       <c r="K134">
         <f>AVERAGE($G$1:G134)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="135" spans="11:11">
       <c r="K135">
         <f>AVERAGE($G$1:G135)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="136" spans="11:11">
       <c r="K136">
         <f>AVERAGE($G$1:G136)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="137" spans="11:11">
       <c r="K137">
         <f>AVERAGE($G$1:G137)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
     <row r="138" spans="11:11">
       <c r="K138">
         <f>AVERAGE($G$1:G138)</f>
-        <v>21.128712871287128</v>
+        <v>19.504950495049506</v>
       </c>
     </row>
   </sheetData>
@@ -4074,7 +4078,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+    <sheetView topLeftCell="A50" workbookViewId="0">
       <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
@@ -7427,7 +7431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" workbookViewId="0">
+    <sheetView topLeftCell="A38" workbookViewId="0">
       <selection activeCell="B101" sqref="B101:I101"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Agent code decoupled from the client class. res_average includes now a good example of a learnt camel race
</commit_message>
<xml_diff>
--- a/res_averages.xlsx
+++ b/res_averages.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="-5600" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="25600" yWindow="-5600" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Pacman Test" sheetId="1" r:id="rId1"/>
     <sheet name="Infection Test" sheetId="2" r:id="rId2"/>
     <sheet name="Butterflies Test" sheetId="3" r:id="rId3"/>
     <sheet name="Zelda Test" sheetId="4" r:id="rId4"/>
+    <sheet name="Camel Race" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2025" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2532" uniqueCount="8">
   <si>
     <t>Result</t>
   </si>
@@ -43,6 +44,9 @@
   </si>
   <si>
     <t>To import text: use special paste, selecting comma, : as special character and space for delimitations</t>
+  </si>
+  <si>
+    <t>AVERAGE WINS</t>
   </si>
 </sst>
 </file>
@@ -99,8 +103,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -136,7 +154,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -152,6 +170,13 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -167,6 +192,13 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -498,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B101" sqref="B101:I101"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="F111" sqref="F111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10785,7 +10817,7 @@
   <dimension ref="A1:K101"/>
   <sheetViews>
     <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B101" sqref="B101:I101"/>
+      <selection activeCell="A48" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -14120,6 +14152,3763 @@
       <c r="K101">
         <f>AVERAGE($G$1:G101)</f>
         <v>-8.9108910891089105E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="L103" sqref="L103"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="11" max="11" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1">
+        <v>-1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1">
+        <v>79</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>-1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2">
+        <v>79</v>
+      </c>
+      <c r="K2">
+        <f>AVERAGE($G$1:G2)</f>
+        <v>-1</v>
+      </c>
+      <c r="L2">
+        <f>AVERAGE($E$1:E2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>-1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>79</v>
+      </c>
+      <c r="K3">
+        <f>AVERAGE($G$1:G3)</f>
+        <v>-1</v>
+      </c>
+      <c r="L3">
+        <f>AVERAGE($E$1:E3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>-1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4">
+        <v>79</v>
+      </c>
+      <c r="K4">
+        <f>AVERAGE($G$1:G4)</f>
+        <v>-1</v>
+      </c>
+      <c r="L4">
+        <f>AVERAGE($E$1:E4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>-1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>79</v>
+      </c>
+      <c r="K5">
+        <f>AVERAGE($G$1:G5)</f>
+        <v>-1</v>
+      </c>
+      <c r="L5">
+        <f>AVERAGE($E$1:E5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>-1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>79</v>
+      </c>
+      <c r="K6">
+        <f>AVERAGE($G$1:G6)</f>
+        <v>-1</v>
+      </c>
+      <c r="L6">
+        <f>AVERAGE($E$1:E6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>-1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>79</v>
+      </c>
+      <c r="K7">
+        <f>AVERAGE($G$1:G7)</f>
+        <v>-1</v>
+      </c>
+      <c r="L7">
+        <f>AVERAGE($E$1:E7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <v>-1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8">
+        <v>79</v>
+      </c>
+      <c r="K8">
+        <f>AVERAGE($G$1:G8)</f>
+        <v>-1</v>
+      </c>
+      <c r="L8">
+        <f>AVERAGE($E$1:E8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <v>-1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9">
+        <v>79</v>
+      </c>
+      <c r="K9">
+        <f>AVERAGE($G$1:G9)</f>
+        <v>-1</v>
+      </c>
+      <c r="L9">
+        <f>AVERAGE($E$1:E9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <v>-1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10">
+        <v>79</v>
+      </c>
+      <c r="K10">
+        <f>AVERAGE($G$1:G10)</f>
+        <v>-1</v>
+      </c>
+      <c r="L10">
+        <f>AVERAGE($E$1:E10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11">
+        <v>-1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>79</v>
+      </c>
+      <c r="K11">
+        <f>AVERAGE($G$1:G11)</f>
+        <v>-1</v>
+      </c>
+      <c r="L11">
+        <f>AVERAGE($E$1:E11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12">
+        <v>-1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12">
+        <v>79</v>
+      </c>
+      <c r="K12">
+        <f>AVERAGE($G$1:G12)</f>
+        <v>-1</v>
+      </c>
+      <c r="L12">
+        <f>AVERAGE($E$1:E12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <v>-1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13">
+        <v>79</v>
+      </c>
+      <c r="K13">
+        <f>AVERAGE($G$1:G13)</f>
+        <v>-1</v>
+      </c>
+      <c r="L13">
+        <f>AVERAGE($E$1:E13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>-1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I14">
+        <v>79</v>
+      </c>
+      <c r="K14">
+        <f>AVERAGE($G$1:G14)</f>
+        <v>-1</v>
+      </c>
+      <c r="L14">
+        <f>AVERAGE($E$1:E14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15">
+        <v>-1</v>
+      </c>
+      <c r="H15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15">
+        <v>79</v>
+      </c>
+      <c r="K15">
+        <f>AVERAGE($G$1:G15)</f>
+        <v>-1</v>
+      </c>
+      <c r="L15">
+        <f>AVERAGE($E$1:E15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16">
+        <v>-1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16">
+        <v>79</v>
+      </c>
+      <c r="K16">
+        <f>AVERAGE($G$1:G16)</f>
+        <v>-1</v>
+      </c>
+      <c r="L16">
+        <f>AVERAGE($E$1:E16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17">
+        <v>-1</v>
+      </c>
+      <c r="H17" t="s">
+        <v>4</v>
+      </c>
+      <c r="I17">
+        <v>79</v>
+      </c>
+      <c r="K17">
+        <f>AVERAGE($G$1:G17)</f>
+        <v>-1</v>
+      </c>
+      <c r="L17">
+        <f>AVERAGE($E$1:E17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18">
+        <v>-1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>4</v>
+      </c>
+      <c r="I18">
+        <v>79</v>
+      </c>
+      <c r="K18">
+        <f>AVERAGE($G$1:G18)</f>
+        <v>-1</v>
+      </c>
+      <c r="L18">
+        <f>AVERAGE($E$1:E18)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19">
+        <v>-1</v>
+      </c>
+      <c r="H19" t="s">
+        <v>4</v>
+      </c>
+      <c r="I19">
+        <v>79</v>
+      </c>
+      <c r="K19">
+        <f>AVERAGE($G$1:G19)</f>
+        <v>-1</v>
+      </c>
+      <c r="L19">
+        <f>AVERAGE($E$1:E19)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20">
+        <v>-1</v>
+      </c>
+      <c r="H20" t="s">
+        <v>4</v>
+      </c>
+      <c r="I20">
+        <v>79</v>
+      </c>
+      <c r="K20">
+        <f>AVERAGE($G$1:G20)</f>
+        <v>-1</v>
+      </c>
+      <c r="L20">
+        <f>AVERAGE($E$1:E20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21">
+        <v>-1</v>
+      </c>
+      <c r="H21" t="s">
+        <v>4</v>
+      </c>
+      <c r="I21">
+        <v>79</v>
+      </c>
+      <c r="K21">
+        <f>AVERAGE($G$1:G21)</f>
+        <v>-1</v>
+      </c>
+      <c r="L21">
+        <f>AVERAGE($E$1:E21)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22">
+        <v>-1</v>
+      </c>
+      <c r="H22" t="s">
+        <v>4</v>
+      </c>
+      <c r="I22">
+        <v>79</v>
+      </c>
+      <c r="K22">
+        <f>AVERAGE($G$1:G22)</f>
+        <v>-1</v>
+      </c>
+      <c r="L22">
+        <f>AVERAGE($E$1:E22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23">
+        <v>-1</v>
+      </c>
+      <c r="H23" t="s">
+        <v>4</v>
+      </c>
+      <c r="I23">
+        <v>79</v>
+      </c>
+      <c r="K23">
+        <f>AVERAGE($G$1:G23)</f>
+        <v>-1</v>
+      </c>
+      <c r="L23">
+        <f>AVERAGE($E$1:E23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24">
+        <v>-1</v>
+      </c>
+      <c r="H24" t="s">
+        <v>4</v>
+      </c>
+      <c r="I24">
+        <v>79</v>
+      </c>
+      <c r="K24">
+        <f>AVERAGE($G$1:G24)</f>
+        <v>-1</v>
+      </c>
+      <c r="L24">
+        <f>AVERAGE($E$1:E24)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25">
+        <v>-1</v>
+      </c>
+      <c r="H25" t="s">
+        <v>4</v>
+      </c>
+      <c r="I25">
+        <v>79</v>
+      </c>
+      <c r="K25">
+        <f>AVERAGE($G$1:G25)</f>
+        <v>-1</v>
+      </c>
+      <c r="L25">
+        <f>AVERAGE($E$1:E25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26">
+        <v>-1</v>
+      </c>
+      <c r="H26" t="s">
+        <v>4</v>
+      </c>
+      <c r="I26">
+        <v>79</v>
+      </c>
+      <c r="K26">
+        <f>AVERAGE($G$1:G26)</f>
+        <v>-1</v>
+      </c>
+      <c r="L26">
+        <f>AVERAGE($E$1:E26)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27" t="s">
+        <v>4</v>
+      </c>
+      <c r="I27">
+        <v>50</v>
+      </c>
+      <c r="K27">
+        <f>AVERAGE($G$1:G27)</f>
+        <v>-0.92592592592592593</v>
+      </c>
+      <c r="L27">
+        <f>AVERAGE($E$1:E27)</f>
+        <v>3.7037037037037035E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28">
+        <v>-1</v>
+      </c>
+      <c r="H28" t="s">
+        <v>4</v>
+      </c>
+      <c r="I28">
+        <v>79</v>
+      </c>
+      <c r="K28">
+        <f>AVERAGE($G$1:G28)</f>
+        <v>-0.9285714285714286</v>
+      </c>
+      <c r="L28">
+        <f>AVERAGE($E$1:E28)</f>
+        <v>3.5714285714285712E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29">
+        <v>-1</v>
+      </c>
+      <c r="H29" t="s">
+        <v>4</v>
+      </c>
+      <c r="I29">
+        <v>79</v>
+      </c>
+      <c r="K29">
+        <f>AVERAGE($G$1:G29)</f>
+        <v>-0.93103448275862066</v>
+      </c>
+      <c r="L29">
+        <f>AVERAGE($E$1:E29)</f>
+        <v>3.4482758620689655E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30">
+        <v>-1</v>
+      </c>
+      <c r="H30" t="s">
+        <v>4</v>
+      </c>
+      <c r="I30">
+        <v>79</v>
+      </c>
+      <c r="K30">
+        <f>AVERAGE($G$1:G30)</f>
+        <v>-0.93333333333333335</v>
+      </c>
+      <c r="L30">
+        <f>AVERAGE($E$1:E30)</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31">
+        <v>-1</v>
+      </c>
+      <c r="H31" t="s">
+        <v>4</v>
+      </c>
+      <c r="I31">
+        <v>79</v>
+      </c>
+      <c r="K31">
+        <f>AVERAGE($G$1:G31)</f>
+        <v>-0.93548387096774188</v>
+      </c>
+      <c r="L31">
+        <f>AVERAGE($E$1:E31)</f>
+        <v>3.2258064516129031E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>2</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32" t="s">
+        <v>3</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32" t="s">
+        <v>4</v>
+      </c>
+      <c r="I32">
+        <v>52</v>
+      </c>
+      <c r="K32">
+        <f>AVERAGE($G$1:G32)</f>
+        <v>-0.875</v>
+      </c>
+      <c r="L32">
+        <f>AVERAGE($E$1:E32)</f>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>2</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33" t="s">
+        <v>3</v>
+      </c>
+      <c r="G33">
+        <v>-1</v>
+      </c>
+      <c r="H33" t="s">
+        <v>4</v>
+      </c>
+      <c r="I33">
+        <v>79</v>
+      </c>
+      <c r="K33">
+        <f>AVERAGE($G$1:G33)</f>
+        <v>-0.87878787878787878</v>
+      </c>
+      <c r="L33">
+        <f>AVERAGE($E$1:E33)</f>
+        <v>6.0606060606060608E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34" t="s">
+        <v>3</v>
+      </c>
+      <c r="G34">
+        <v>-1</v>
+      </c>
+      <c r="H34" t="s">
+        <v>4</v>
+      </c>
+      <c r="I34">
+        <v>79</v>
+      </c>
+      <c r="K34">
+        <f>AVERAGE($G$1:G34)</f>
+        <v>-0.88235294117647056</v>
+      </c>
+      <c r="L34">
+        <f>AVERAGE($E$1:E34)</f>
+        <v>5.8823529411764705E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>2</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35" t="s">
+        <v>3</v>
+      </c>
+      <c r="G35">
+        <v>-1</v>
+      </c>
+      <c r="H35" t="s">
+        <v>4</v>
+      </c>
+      <c r="I35">
+        <v>79</v>
+      </c>
+      <c r="K35">
+        <f>AVERAGE($G$1:G35)</f>
+        <v>-0.88571428571428568</v>
+      </c>
+      <c r="L35">
+        <f>AVERAGE($E$1:E35)</f>
+        <v>5.7142857142857141E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>2</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36" t="s">
+        <v>3</v>
+      </c>
+      <c r="G36">
+        <v>-1</v>
+      </c>
+      <c r="H36" t="s">
+        <v>4</v>
+      </c>
+      <c r="I36">
+        <v>79</v>
+      </c>
+      <c r="K36">
+        <f>AVERAGE($G$1:G36)</f>
+        <v>-0.88888888888888884</v>
+      </c>
+      <c r="L36">
+        <f>AVERAGE($E$1:E36)</f>
+        <v>5.5555555555555552E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>2</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37" t="s">
+        <v>3</v>
+      </c>
+      <c r="G37">
+        <v>-1</v>
+      </c>
+      <c r="H37" t="s">
+        <v>4</v>
+      </c>
+      <c r="I37">
+        <v>79</v>
+      </c>
+      <c r="K37">
+        <f>AVERAGE($G$1:G37)</f>
+        <v>-0.89189189189189189</v>
+      </c>
+      <c r="L37">
+        <f>AVERAGE($E$1:E37)</f>
+        <v>5.4054054054054057E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38" t="s">
+        <v>3</v>
+      </c>
+      <c r="G38">
+        <v>-1</v>
+      </c>
+      <c r="H38" t="s">
+        <v>4</v>
+      </c>
+      <c r="I38">
+        <v>79</v>
+      </c>
+      <c r="K38">
+        <f>AVERAGE($G$1:G38)</f>
+        <v>-0.89473684210526316</v>
+      </c>
+      <c r="L38">
+        <f>AVERAGE($E$1:E38)</f>
+        <v>5.2631578947368418E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>2</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39" t="s">
+        <v>3</v>
+      </c>
+      <c r="G39">
+        <v>-1</v>
+      </c>
+      <c r="H39" t="s">
+        <v>4</v>
+      </c>
+      <c r="I39">
+        <v>79</v>
+      </c>
+      <c r="K39">
+        <f>AVERAGE($G$1:G39)</f>
+        <v>-0.89743589743589747</v>
+      </c>
+      <c r="L39">
+        <f>AVERAGE($E$1:E39)</f>
+        <v>5.128205128205128E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>2</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40" t="s">
+        <v>3</v>
+      </c>
+      <c r="G40">
+        <v>-1</v>
+      </c>
+      <c r="H40" t="s">
+        <v>4</v>
+      </c>
+      <c r="I40">
+        <v>79</v>
+      </c>
+      <c r="K40">
+        <f>AVERAGE($G$1:G40)</f>
+        <v>-0.9</v>
+      </c>
+      <c r="L40">
+        <f>AVERAGE($E$1:E40)</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
+        <v>2</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41" t="s">
+        <v>3</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41" t="s">
+        <v>4</v>
+      </c>
+      <c r="I41">
+        <v>54</v>
+      </c>
+      <c r="K41">
+        <f>AVERAGE($G$1:G41)</f>
+        <v>-0.85365853658536583</v>
+      </c>
+      <c r="L41">
+        <f>AVERAGE($E$1:E41)</f>
+        <v>7.3170731707317069E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
+        <v>2</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42" t="s">
+        <v>3</v>
+      </c>
+      <c r="G42">
+        <v>-1</v>
+      </c>
+      <c r="H42" t="s">
+        <v>4</v>
+      </c>
+      <c r="I42">
+        <v>79</v>
+      </c>
+      <c r="K42">
+        <f>AVERAGE($G$1:G42)</f>
+        <v>-0.8571428571428571</v>
+      </c>
+      <c r="L42">
+        <f>AVERAGE($E$1:E42)</f>
+        <v>7.1428571428571425E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>2</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43" t="s">
+        <v>3</v>
+      </c>
+      <c r="G43">
+        <v>-1</v>
+      </c>
+      <c r="H43" t="s">
+        <v>4</v>
+      </c>
+      <c r="I43">
+        <v>79</v>
+      </c>
+      <c r="K43">
+        <f>AVERAGE($G$1:G43)</f>
+        <v>-0.86046511627906974</v>
+      </c>
+      <c r="L43">
+        <f>AVERAGE($E$1:E43)</f>
+        <v>6.9767441860465115E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1</v>
+      </c>
+      <c r="D44" t="s">
+        <v>2</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44" t="s">
+        <v>3</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44" t="s">
+        <v>4</v>
+      </c>
+      <c r="I44">
+        <v>51</v>
+      </c>
+      <c r="K44">
+        <f>AVERAGE($G$1:G44)</f>
+        <v>-0.81818181818181823</v>
+      </c>
+      <c r="L44">
+        <f>AVERAGE($E$1:E44)</f>
+        <v>9.0909090909090912E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1</v>
+      </c>
+      <c r="D45" t="s">
+        <v>2</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45" t="s">
+        <v>3</v>
+      </c>
+      <c r="G45">
+        <v>-1</v>
+      </c>
+      <c r="H45" t="s">
+        <v>4</v>
+      </c>
+      <c r="I45">
+        <v>79</v>
+      </c>
+      <c r="K45">
+        <f>AVERAGE($G$1:G45)</f>
+        <v>-0.82222222222222219</v>
+      </c>
+      <c r="L45">
+        <f>AVERAGE($E$1:E45)</f>
+        <v>8.8888888888888892E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1</v>
+      </c>
+      <c r="D46" t="s">
+        <v>2</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46" t="s">
+        <v>3</v>
+      </c>
+      <c r="G46">
+        <v>-1</v>
+      </c>
+      <c r="H46" t="s">
+        <v>4</v>
+      </c>
+      <c r="I46">
+        <v>79</v>
+      </c>
+      <c r="K46">
+        <f>AVERAGE($G$1:G46)</f>
+        <v>-0.82608695652173914</v>
+      </c>
+      <c r="L46">
+        <f>AVERAGE($E$1:E46)</f>
+        <v>8.6956521739130432E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1</v>
+      </c>
+      <c r="D47" t="s">
+        <v>2</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47" t="s">
+        <v>3</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+      <c r="H47" t="s">
+        <v>4</v>
+      </c>
+      <c r="I47">
+        <v>47</v>
+      </c>
+      <c r="K47">
+        <f>AVERAGE($G$1:G47)</f>
+        <v>-0.78723404255319152</v>
+      </c>
+      <c r="L47">
+        <f>AVERAGE($E$1:E47)</f>
+        <v>0.10638297872340426</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1</v>
+      </c>
+      <c r="D48" t="s">
+        <v>2</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48" t="s">
+        <v>3</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+      <c r="H48" t="s">
+        <v>4</v>
+      </c>
+      <c r="I48">
+        <v>48</v>
+      </c>
+      <c r="K48">
+        <f>AVERAGE($G$1:G48)</f>
+        <v>-0.75</v>
+      </c>
+      <c r="L48">
+        <f>AVERAGE($E$1:E48)</f>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" t="s">
+        <v>1</v>
+      </c>
+      <c r="D49" t="s">
+        <v>2</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49" t="s">
+        <v>3</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+      <c r="H49" t="s">
+        <v>4</v>
+      </c>
+      <c r="I49">
+        <v>51</v>
+      </c>
+      <c r="K49">
+        <f>AVERAGE($G$1:G49)</f>
+        <v>-0.7142857142857143</v>
+      </c>
+      <c r="L49">
+        <f>AVERAGE($E$1:E49)</f>
+        <v>0.14285714285714285</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50" t="s">
+        <v>2</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50" t="s">
+        <v>3</v>
+      </c>
+      <c r="G50">
+        <v>-1</v>
+      </c>
+      <c r="H50" t="s">
+        <v>4</v>
+      </c>
+      <c r="I50">
+        <v>79</v>
+      </c>
+      <c r="K50">
+        <f>AVERAGE($G$1:G50)</f>
+        <v>-0.72</v>
+      </c>
+      <c r="L50">
+        <f>AVERAGE($E$1:E50)</f>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" t="s">
+        <v>1</v>
+      </c>
+      <c r="D51" t="s">
+        <v>2</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51" t="s">
+        <v>3</v>
+      </c>
+      <c r="G51">
+        <v>-1</v>
+      </c>
+      <c r="H51" t="s">
+        <v>4</v>
+      </c>
+      <c r="I51">
+        <v>79</v>
+      </c>
+      <c r="K51">
+        <f>AVERAGE($G$1:G51)</f>
+        <v>-0.72549019607843135</v>
+      </c>
+      <c r="L51">
+        <f>AVERAGE($E$1:E51)</f>
+        <v>0.13725490196078433</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" t="s">
+        <v>1</v>
+      </c>
+      <c r="D52" t="s">
+        <v>2</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52" t="s">
+        <v>3</v>
+      </c>
+      <c r="G52">
+        <v>-1</v>
+      </c>
+      <c r="H52" t="s">
+        <v>4</v>
+      </c>
+      <c r="I52">
+        <v>79</v>
+      </c>
+      <c r="K52">
+        <f>AVERAGE($G$1:G52)</f>
+        <v>-0.73076923076923073</v>
+      </c>
+      <c r="L52">
+        <f>AVERAGE($E$1:E52)</f>
+        <v>0.13461538461538461</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53" t="s">
+        <v>1</v>
+      </c>
+      <c r="D53" t="s">
+        <v>2</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53" t="s">
+        <v>3</v>
+      </c>
+      <c r="G53">
+        <v>-1</v>
+      </c>
+      <c r="H53" t="s">
+        <v>4</v>
+      </c>
+      <c r="I53">
+        <v>79</v>
+      </c>
+      <c r="K53">
+        <f>AVERAGE($G$1:G53)</f>
+        <v>-0.73584905660377353</v>
+      </c>
+      <c r="L53">
+        <f>AVERAGE($E$1:E53)</f>
+        <v>0.13207547169811321</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>0</v>
+      </c>
+      <c r="C54" t="s">
+        <v>1</v>
+      </c>
+      <c r="D54" t="s">
+        <v>2</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54" t="s">
+        <v>3</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="H54" t="s">
+        <v>4</v>
+      </c>
+      <c r="I54">
+        <v>47</v>
+      </c>
+      <c r="K54">
+        <f>AVERAGE($G$1:G54)</f>
+        <v>-0.70370370370370372</v>
+      </c>
+      <c r="L54">
+        <f>AVERAGE($E$1:E54)</f>
+        <v>0.14814814814814814</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>0</v>
+      </c>
+      <c r="C55" t="s">
+        <v>1</v>
+      </c>
+      <c r="D55" t="s">
+        <v>2</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55" t="s">
+        <v>3</v>
+      </c>
+      <c r="G55">
+        <v>-1</v>
+      </c>
+      <c r="H55" t="s">
+        <v>4</v>
+      </c>
+      <c r="I55">
+        <v>79</v>
+      </c>
+      <c r="K55">
+        <f>AVERAGE($G$1:G55)</f>
+        <v>-0.70909090909090911</v>
+      </c>
+      <c r="L55">
+        <f>AVERAGE($E$1:E55)</f>
+        <v>0.14545454545454545</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>0</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1</v>
+      </c>
+      <c r="D56" t="s">
+        <v>2</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56" t="s">
+        <v>3</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56" t="s">
+        <v>4</v>
+      </c>
+      <c r="I56">
+        <v>52</v>
+      </c>
+      <c r="K56">
+        <f>AVERAGE($G$1:G56)</f>
+        <v>-0.6785714285714286</v>
+      </c>
+      <c r="L56">
+        <f>AVERAGE($E$1:E56)</f>
+        <v>0.16071428571428573</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" t="s">
+        <v>1</v>
+      </c>
+      <c r="D57" t="s">
+        <v>2</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57" t="s">
+        <v>3</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="H57" t="s">
+        <v>4</v>
+      </c>
+      <c r="I57">
+        <v>54</v>
+      </c>
+      <c r="K57">
+        <f>AVERAGE($G$1:G57)</f>
+        <v>-0.64912280701754388</v>
+      </c>
+      <c r="L57">
+        <f>AVERAGE($E$1:E57)</f>
+        <v>0.17543859649122806</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>0</v>
+      </c>
+      <c r="C58" t="s">
+        <v>1</v>
+      </c>
+      <c r="D58" t="s">
+        <v>2</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58" t="s">
+        <v>3</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+      <c r="H58" t="s">
+        <v>4</v>
+      </c>
+      <c r="I58">
+        <v>50</v>
+      </c>
+      <c r="K58">
+        <f>AVERAGE($G$1:G58)</f>
+        <v>-0.62068965517241381</v>
+      </c>
+      <c r="L58">
+        <f>AVERAGE($E$1:E58)</f>
+        <v>0.18965517241379309</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" t="s">
+        <v>1</v>
+      </c>
+      <c r="D59" t="s">
+        <v>2</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59" t="s">
+        <v>3</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59" t="s">
+        <v>4</v>
+      </c>
+      <c r="I59">
+        <v>50</v>
+      </c>
+      <c r="K59">
+        <f>AVERAGE($G$1:G59)</f>
+        <v>-0.59322033898305082</v>
+      </c>
+      <c r="L59">
+        <f>AVERAGE($E$1:E59)</f>
+        <v>0.20338983050847459</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>0</v>
+      </c>
+      <c r="C60" t="s">
+        <v>1</v>
+      </c>
+      <c r="D60" t="s">
+        <v>2</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60" t="s">
+        <v>3</v>
+      </c>
+      <c r="G60">
+        <v>-1</v>
+      </c>
+      <c r="H60" t="s">
+        <v>4</v>
+      </c>
+      <c r="I60">
+        <v>79</v>
+      </c>
+      <c r="K60">
+        <f>AVERAGE($G$1:G60)</f>
+        <v>-0.6</v>
+      </c>
+      <c r="L60">
+        <f>AVERAGE($E$1:E60)</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>0</v>
+      </c>
+      <c r="C61" t="s">
+        <v>1</v>
+      </c>
+      <c r="D61" t="s">
+        <v>2</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61" t="s">
+        <v>3</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
+      <c r="H61" t="s">
+        <v>4</v>
+      </c>
+      <c r="I61">
+        <v>46</v>
+      </c>
+      <c r="K61">
+        <f>AVERAGE($G$1:G61)</f>
+        <v>-0.57377049180327866</v>
+      </c>
+      <c r="L61">
+        <f>AVERAGE($E$1:E61)</f>
+        <v>0.21311475409836064</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>0</v>
+      </c>
+      <c r="C62" t="s">
+        <v>1</v>
+      </c>
+      <c r="D62" t="s">
+        <v>2</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62" t="s">
+        <v>3</v>
+      </c>
+      <c r="G62">
+        <v>1</v>
+      </c>
+      <c r="H62" t="s">
+        <v>4</v>
+      </c>
+      <c r="I62">
+        <v>54</v>
+      </c>
+      <c r="K62">
+        <f>AVERAGE($G$1:G62)</f>
+        <v>-0.54838709677419351</v>
+      </c>
+      <c r="L62">
+        <f>AVERAGE($E$1:E62)</f>
+        <v>0.22580645161290322</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>0</v>
+      </c>
+      <c r="C63" t="s">
+        <v>1</v>
+      </c>
+      <c r="D63" t="s">
+        <v>2</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63" t="s">
+        <v>3</v>
+      </c>
+      <c r="G63">
+        <v>1</v>
+      </c>
+      <c r="H63" t="s">
+        <v>4</v>
+      </c>
+      <c r="I63">
+        <v>53</v>
+      </c>
+      <c r="K63">
+        <f>AVERAGE($G$1:G63)</f>
+        <v>-0.52380952380952384</v>
+      </c>
+      <c r="L63">
+        <f>AVERAGE($E$1:E63)</f>
+        <v>0.23809523809523808</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>0</v>
+      </c>
+      <c r="C64" t="s">
+        <v>1</v>
+      </c>
+      <c r="D64" t="s">
+        <v>2</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64" t="s">
+        <v>3</v>
+      </c>
+      <c r="G64">
+        <v>1</v>
+      </c>
+      <c r="H64" t="s">
+        <v>4</v>
+      </c>
+      <c r="I64">
+        <v>52</v>
+      </c>
+      <c r="K64">
+        <f>AVERAGE($G$1:G64)</f>
+        <v>-0.5</v>
+      </c>
+      <c r="L64">
+        <f>AVERAGE($E$1:E64)</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>0</v>
+      </c>
+      <c r="C65" t="s">
+        <v>1</v>
+      </c>
+      <c r="D65" t="s">
+        <v>2</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="F65" t="s">
+        <v>3</v>
+      </c>
+      <c r="G65">
+        <v>1</v>
+      </c>
+      <c r="H65" t="s">
+        <v>4</v>
+      </c>
+      <c r="I65">
+        <v>52</v>
+      </c>
+      <c r="K65">
+        <f>AVERAGE($G$1:G65)</f>
+        <v>-0.47692307692307695</v>
+      </c>
+      <c r="L65">
+        <f>AVERAGE($E$1:E65)</f>
+        <v>0.26153846153846155</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>0</v>
+      </c>
+      <c r="C66" t="s">
+        <v>1</v>
+      </c>
+      <c r="D66" t="s">
+        <v>2</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66" t="s">
+        <v>3</v>
+      </c>
+      <c r="G66">
+        <v>1</v>
+      </c>
+      <c r="H66" t="s">
+        <v>4</v>
+      </c>
+      <c r="I66">
+        <v>50</v>
+      </c>
+      <c r="K66">
+        <f>AVERAGE($G$1:G66)</f>
+        <v>-0.45454545454545453</v>
+      </c>
+      <c r="L66">
+        <f>AVERAGE($E$1:E66)</f>
+        <v>0.27272727272727271</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>0</v>
+      </c>
+      <c r="C67" t="s">
+        <v>1</v>
+      </c>
+      <c r="D67" t="s">
+        <v>2</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="F67" t="s">
+        <v>3</v>
+      </c>
+      <c r="G67">
+        <v>1</v>
+      </c>
+      <c r="H67" t="s">
+        <v>4</v>
+      </c>
+      <c r="I67">
+        <v>49</v>
+      </c>
+      <c r="K67">
+        <f>AVERAGE($G$1:G67)</f>
+        <v>-0.43283582089552236</v>
+      </c>
+      <c r="L67">
+        <f>AVERAGE($E$1:E67)</f>
+        <v>0.28358208955223879</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>0</v>
+      </c>
+      <c r="C68" t="s">
+        <v>1</v>
+      </c>
+      <c r="D68" t="s">
+        <v>2</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68" t="s">
+        <v>3</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
+      <c r="H68" t="s">
+        <v>4</v>
+      </c>
+      <c r="I68">
+        <v>50</v>
+      </c>
+      <c r="K68">
+        <f>AVERAGE($G$1:G68)</f>
+        <v>-0.41176470588235292</v>
+      </c>
+      <c r="L68">
+        <f>AVERAGE($E$1:E68)</f>
+        <v>0.29411764705882354</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>0</v>
+      </c>
+      <c r="C69" t="s">
+        <v>1</v>
+      </c>
+      <c r="D69" t="s">
+        <v>2</v>
+      </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
+      <c r="F69" t="s">
+        <v>3</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+      <c r="H69" t="s">
+        <v>4</v>
+      </c>
+      <c r="I69">
+        <v>55</v>
+      </c>
+      <c r="K69">
+        <f>AVERAGE($G$1:G69)</f>
+        <v>-0.39130434782608697</v>
+      </c>
+      <c r="L69">
+        <f>AVERAGE($E$1:E69)</f>
+        <v>0.30434782608695654</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>0</v>
+      </c>
+      <c r="C70" t="s">
+        <v>1</v>
+      </c>
+      <c r="D70" t="s">
+        <v>2</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70" t="s">
+        <v>3</v>
+      </c>
+      <c r="G70">
+        <v>-1</v>
+      </c>
+      <c r="H70" t="s">
+        <v>4</v>
+      </c>
+      <c r="I70">
+        <v>79</v>
+      </c>
+      <c r="K70">
+        <f>AVERAGE($G$1:G70)</f>
+        <v>-0.4</v>
+      </c>
+      <c r="L70">
+        <f>AVERAGE($E$1:E70)</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>0</v>
+      </c>
+      <c r="C71" t="s">
+        <v>1</v>
+      </c>
+      <c r="D71" t="s">
+        <v>2</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="F71" t="s">
+        <v>3</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
+      </c>
+      <c r="H71" t="s">
+        <v>4</v>
+      </c>
+      <c r="I71">
+        <v>53</v>
+      </c>
+      <c r="K71">
+        <f>AVERAGE($G$1:G71)</f>
+        <v>-0.38028169014084506</v>
+      </c>
+      <c r="L71">
+        <f>AVERAGE($E$1:E71)</f>
+        <v>0.30985915492957744</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>0</v>
+      </c>
+      <c r="C72" t="s">
+        <v>1</v>
+      </c>
+      <c r="D72" t="s">
+        <v>2</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+      <c r="F72" t="s">
+        <v>3</v>
+      </c>
+      <c r="G72">
+        <v>1</v>
+      </c>
+      <c r="H72" t="s">
+        <v>4</v>
+      </c>
+      <c r="I72">
+        <v>49</v>
+      </c>
+      <c r="K72">
+        <f>AVERAGE($G$1:G72)</f>
+        <v>-0.3611111111111111</v>
+      </c>
+      <c r="L72">
+        <f>AVERAGE($E$1:E72)</f>
+        <v>0.31944444444444442</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>0</v>
+      </c>
+      <c r="C73" t="s">
+        <v>1</v>
+      </c>
+      <c r="D73" t="s">
+        <v>2</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="F73" t="s">
+        <v>3</v>
+      </c>
+      <c r="G73">
+        <v>1</v>
+      </c>
+      <c r="H73" t="s">
+        <v>4</v>
+      </c>
+      <c r="I73">
+        <v>54</v>
+      </c>
+      <c r="K73">
+        <f>AVERAGE($G$1:G73)</f>
+        <v>-0.34246575342465752</v>
+      </c>
+      <c r="L73">
+        <f>AVERAGE($E$1:E73)</f>
+        <v>0.32876712328767121</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>0</v>
+      </c>
+      <c r="C74" t="s">
+        <v>1</v>
+      </c>
+      <c r="D74" t="s">
+        <v>2</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="F74" t="s">
+        <v>3</v>
+      </c>
+      <c r="G74">
+        <v>1</v>
+      </c>
+      <c r="H74" t="s">
+        <v>4</v>
+      </c>
+      <c r="I74">
+        <v>50</v>
+      </c>
+      <c r="K74">
+        <f>AVERAGE($G$1:G74)</f>
+        <v>-0.32432432432432434</v>
+      </c>
+      <c r="L74">
+        <f>AVERAGE($E$1:E74)</f>
+        <v>0.33783783783783783</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>0</v>
+      </c>
+      <c r="C75" t="s">
+        <v>1</v>
+      </c>
+      <c r="D75" t="s">
+        <v>2</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75" t="s">
+        <v>3</v>
+      </c>
+      <c r="G75">
+        <v>-1</v>
+      </c>
+      <c r="H75" t="s">
+        <v>4</v>
+      </c>
+      <c r="I75">
+        <v>79</v>
+      </c>
+      <c r="K75">
+        <f>AVERAGE($G$1:G75)</f>
+        <v>-0.33333333333333331</v>
+      </c>
+      <c r="L75">
+        <f>AVERAGE($E$1:E75)</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>0</v>
+      </c>
+      <c r="C76" t="s">
+        <v>1</v>
+      </c>
+      <c r="D76" t="s">
+        <v>2</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="F76" t="s">
+        <v>3</v>
+      </c>
+      <c r="G76">
+        <v>1</v>
+      </c>
+      <c r="H76" t="s">
+        <v>4</v>
+      </c>
+      <c r="I76">
+        <v>49</v>
+      </c>
+      <c r="K76">
+        <f>AVERAGE($G$1:G76)</f>
+        <v>-0.31578947368421051</v>
+      </c>
+      <c r="L76">
+        <f>AVERAGE($E$1:E76)</f>
+        <v>0.34210526315789475</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>0</v>
+      </c>
+      <c r="C77" t="s">
+        <v>1</v>
+      </c>
+      <c r="D77" t="s">
+        <v>2</v>
+      </c>
+      <c r="E77">
+        <v>1</v>
+      </c>
+      <c r="F77" t="s">
+        <v>3</v>
+      </c>
+      <c r="G77">
+        <v>1</v>
+      </c>
+      <c r="H77" t="s">
+        <v>4</v>
+      </c>
+      <c r="I77">
+        <v>53</v>
+      </c>
+      <c r="K77">
+        <f>AVERAGE($G$1:G77)</f>
+        <v>-0.29870129870129869</v>
+      </c>
+      <c r="L77">
+        <f>AVERAGE($E$1:E77)</f>
+        <v>0.35064935064935066</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>0</v>
+      </c>
+      <c r="C78" t="s">
+        <v>1</v>
+      </c>
+      <c r="D78" t="s">
+        <v>2</v>
+      </c>
+      <c r="E78">
+        <v>1</v>
+      </c>
+      <c r="F78" t="s">
+        <v>3</v>
+      </c>
+      <c r="G78">
+        <v>1</v>
+      </c>
+      <c r="H78" t="s">
+        <v>4</v>
+      </c>
+      <c r="I78">
+        <v>51</v>
+      </c>
+      <c r="K78">
+        <f>AVERAGE($G$1:G78)</f>
+        <v>-0.28205128205128205</v>
+      </c>
+      <c r="L78">
+        <f>AVERAGE($E$1:E78)</f>
+        <v>0.35897435897435898</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>0</v>
+      </c>
+      <c r="C79" t="s">
+        <v>1</v>
+      </c>
+      <c r="D79" t="s">
+        <v>2</v>
+      </c>
+      <c r="E79">
+        <v>1</v>
+      </c>
+      <c r="F79" t="s">
+        <v>3</v>
+      </c>
+      <c r="G79">
+        <v>1</v>
+      </c>
+      <c r="H79" t="s">
+        <v>4</v>
+      </c>
+      <c r="I79">
+        <v>49</v>
+      </c>
+      <c r="K79">
+        <f>AVERAGE($G$1:G79)</f>
+        <v>-0.26582278481012656</v>
+      </c>
+      <c r="L79">
+        <f>AVERAGE($E$1:E79)</f>
+        <v>0.36708860759493672</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>0</v>
+      </c>
+      <c r="C80" t="s">
+        <v>1</v>
+      </c>
+      <c r="D80" t="s">
+        <v>2</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80" t="s">
+        <v>3</v>
+      </c>
+      <c r="G80">
+        <v>-1</v>
+      </c>
+      <c r="H80" t="s">
+        <v>4</v>
+      </c>
+      <c r="I80">
+        <v>79</v>
+      </c>
+      <c r="K80">
+        <f>AVERAGE($G$1:G80)</f>
+        <v>-0.27500000000000002</v>
+      </c>
+      <c r="L80">
+        <f>AVERAGE($E$1:E80)</f>
+        <v>0.36249999999999999</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>0</v>
+      </c>
+      <c r="C81" t="s">
+        <v>1</v>
+      </c>
+      <c r="D81" t="s">
+        <v>2</v>
+      </c>
+      <c r="E81">
+        <v>1</v>
+      </c>
+      <c r="F81" t="s">
+        <v>3</v>
+      </c>
+      <c r="G81">
+        <v>1</v>
+      </c>
+      <c r="H81" t="s">
+        <v>4</v>
+      </c>
+      <c r="I81">
+        <v>50</v>
+      </c>
+      <c r="K81">
+        <f>AVERAGE($G$1:G81)</f>
+        <v>-0.25925925925925924</v>
+      </c>
+      <c r="L81">
+        <f>AVERAGE($E$1:E81)</f>
+        <v>0.37037037037037035</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>0</v>
+      </c>
+      <c r="C82" t="s">
+        <v>1</v>
+      </c>
+      <c r="D82" t="s">
+        <v>2</v>
+      </c>
+      <c r="E82">
+        <v>1</v>
+      </c>
+      <c r="F82" t="s">
+        <v>3</v>
+      </c>
+      <c r="G82">
+        <v>1</v>
+      </c>
+      <c r="H82" t="s">
+        <v>4</v>
+      </c>
+      <c r="I82">
+        <v>48</v>
+      </c>
+      <c r="K82">
+        <f>AVERAGE($G$1:G82)</f>
+        <v>-0.24390243902439024</v>
+      </c>
+      <c r="L82">
+        <f>AVERAGE($E$1:E82)</f>
+        <v>0.37804878048780488</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>0</v>
+      </c>
+      <c r="C83" t="s">
+        <v>1</v>
+      </c>
+      <c r="D83" t="s">
+        <v>2</v>
+      </c>
+      <c r="E83">
+        <v>1</v>
+      </c>
+      <c r="F83" t="s">
+        <v>3</v>
+      </c>
+      <c r="G83">
+        <v>1</v>
+      </c>
+      <c r="H83" t="s">
+        <v>4</v>
+      </c>
+      <c r="I83">
+        <v>51</v>
+      </c>
+      <c r="K83">
+        <f>AVERAGE($G$1:G83)</f>
+        <v>-0.2289156626506024</v>
+      </c>
+      <c r="L83">
+        <f>AVERAGE($E$1:E83)</f>
+        <v>0.38554216867469882</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>0</v>
+      </c>
+      <c r="C84" t="s">
+        <v>1</v>
+      </c>
+      <c r="D84" t="s">
+        <v>2</v>
+      </c>
+      <c r="E84">
+        <v>1</v>
+      </c>
+      <c r="F84" t="s">
+        <v>3</v>
+      </c>
+      <c r="G84">
+        <v>1</v>
+      </c>
+      <c r="H84" t="s">
+        <v>4</v>
+      </c>
+      <c r="I84">
+        <v>48</v>
+      </c>
+      <c r="K84">
+        <f>AVERAGE($G$1:G84)</f>
+        <v>-0.21428571428571427</v>
+      </c>
+      <c r="L84">
+        <f>AVERAGE($E$1:E84)</f>
+        <v>0.39285714285714285</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>0</v>
+      </c>
+      <c r="C85" t="s">
+        <v>1</v>
+      </c>
+      <c r="D85" t="s">
+        <v>2</v>
+      </c>
+      <c r="E85">
+        <v>1</v>
+      </c>
+      <c r="F85" t="s">
+        <v>3</v>
+      </c>
+      <c r="G85">
+        <v>1</v>
+      </c>
+      <c r="H85" t="s">
+        <v>4</v>
+      </c>
+      <c r="I85">
+        <v>45</v>
+      </c>
+      <c r="K85">
+        <f>AVERAGE($G$1:G85)</f>
+        <v>-0.2</v>
+      </c>
+      <c r="L85">
+        <f>AVERAGE($E$1:E85)</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>0</v>
+      </c>
+      <c r="C86" t="s">
+        <v>1</v>
+      </c>
+      <c r="D86" t="s">
+        <v>2</v>
+      </c>
+      <c r="E86">
+        <v>0</v>
+      </c>
+      <c r="F86" t="s">
+        <v>3</v>
+      </c>
+      <c r="G86">
+        <v>-1</v>
+      </c>
+      <c r="H86" t="s">
+        <v>4</v>
+      </c>
+      <c r="I86">
+        <v>79</v>
+      </c>
+      <c r="K86">
+        <f>AVERAGE($G$1:G86)</f>
+        <v>-0.20930232558139536</v>
+      </c>
+      <c r="L86">
+        <f>AVERAGE($E$1:E86)</f>
+        <v>0.39534883720930231</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>0</v>
+      </c>
+      <c r="C87" t="s">
+        <v>1</v>
+      </c>
+      <c r="D87" t="s">
+        <v>2</v>
+      </c>
+      <c r="E87">
+        <v>1</v>
+      </c>
+      <c r="F87" t="s">
+        <v>3</v>
+      </c>
+      <c r="G87">
+        <v>1</v>
+      </c>
+      <c r="H87" t="s">
+        <v>4</v>
+      </c>
+      <c r="I87">
+        <v>54</v>
+      </c>
+      <c r="K87">
+        <f>AVERAGE($G$1:G87)</f>
+        <v>-0.19540229885057472</v>
+      </c>
+      <c r="L87">
+        <f>AVERAGE($E$1:E87)</f>
+        <v>0.40229885057471265</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>0</v>
+      </c>
+      <c r="C88" t="s">
+        <v>1</v>
+      </c>
+      <c r="D88" t="s">
+        <v>2</v>
+      </c>
+      <c r="E88">
+        <v>1</v>
+      </c>
+      <c r="F88" t="s">
+        <v>3</v>
+      </c>
+      <c r="G88">
+        <v>1</v>
+      </c>
+      <c r="H88" t="s">
+        <v>4</v>
+      </c>
+      <c r="I88">
+        <v>51</v>
+      </c>
+      <c r="K88">
+        <f>AVERAGE($G$1:G88)</f>
+        <v>-0.18181818181818182</v>
+      </c>
+      <c r="L88">
+        <f>AVERAGE($E$1:E88)</f>
+        <v>0.40909090909090912</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>0</v>
+      </c>
+      <c r="C89" t="s">
+        <v>1</v>
+      </c>
+      <c r="D89" t="s">
+        <v>2</v>
+      </c>
+      <c r="E89">
+        <v>1</v>
+      </c>
+      <c r="F89" t="s">
+        <v>3</v>
+      </c>
+      <c r="G89">
+        <v>1</v>
+      </c>
+      <c r="H89" t="s">
+        <v>4</v>
+      </c>
+      <c r="I89">
+        <v>49</v>
+      </c>
+      <c r="K89">
+        <f>AVERAGE($G$1:G89)</f>
+        <v>-0.16853932584269662</v>
+      </c>
+      <c r="L89">
+        <f>AVERAGE($E$1:E89)</f>
+        <v>0.4157303370786517</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>0</v>
+      </c>
+      <c r="C90" t="s">
+        <v>1</v>
+      </c>
+      <c r="D90" t="s">
+        <v>2</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+      <c r="F90" t="s">
+        <v>3</v>
+      </c>
+      <c r="G90">
+        <v>-1</v>
+      </c>
+      <c r="H90" t="s">
+        <v>4</v>
+      </c>
+      <c r="I90">
+        <v>79</v>
+      </c>
+      <c r="K90">
+        <f>AVERAGE($G$1:G90)</f>
+        <v>-0.17777777777777778</v>
+      </c>
+      <c r="L90">
+        <f>AVERAGE($E$1:E90)</f>
+        <v>0.41111111111111109</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
+        <v>0</v>
+      </c>
+      <c r="C91" t="s">
+        <v>1</v>
+      </c>
+      <c r="D91" t="s">
+        <v>2</v>
+      </c>
+      <c r="E91">
+        <v>1</v>
+      </c>
+      <c r="F91" t="s">
+        <v>3</v>
+      </c>
+      <c r="G91">
+        <v>1</v>
+      </c>
+      <c r="H91" t="s">
+        <v>4</v>
+      </c>
+      <c r="I91">
+        <v>51</v>
+      </c>
+      <c r="K91">
+        <f>AVERAGE($G$1:G91)</f>
+        <v>-0.16483516483516483</v>
+      </c>
+      <c r="L91">
+        <f>AVERAGE($E$1:E91)</f>
+        <v>0.4175824175824176</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>0</v>
+      </c>
+      <c r="C92" t="s">
+        <v>1</v>
+      </c>
+      <c r="D92" t="s">
+        <v>2</v>
+      </c>
+      <c r="E92">
+        <v>1</v>
+      </c>
+      <c r="F92" t="s">
+        <v>3</v>
+      </c>
+      <c r="G92">
+        <v>1</v>
+      </c>
+      <c r="H92" t="s">
+        <v>4</v>
+      </c>
+      <c r="I92">
+        <v>49</v>
+      </c>
+      <c r="K92">
+        <f>AVERAGE($G$1:G92)</f>
+        <v>-0.15217391304347827</v>
+      </c>
+      <c r="L92">
+        <f>AVERAGE($E$1:E92)</f>
+        <v>0.42391304347826086</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>0</v>
+      </c>
+      <c r="C93" t="s">
+        <v>1</v>
+      </c>
+      <c r="D93" t="s">
+        <v>2</v>
+      </c>
+      <c r="E93">
+        <v>1</v>
+      </c>
+      <c r="F93" t="s">
+        <v>3</v>
+      </c>
+      <c r="G93">
+        <v>1</v>
+      </c>
+      <c r="H93" t="s">
+        <v>4</v>
+      </c>
+      <c r="I93">
+        <v>51</v>
+      </c>
+      <c r="K93">
+        <f>AVERAGE($G$1:G93)</f>
+        <v>-0.13978494623655913</v>
+      </c>
+      <c r="L93">
+        <f>AVERAGE($E$1:E93)</f>
+        <v>0.43010752688172044</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>0</v>
+      </c>
+      <c r="C94" t="s">
+        <v>1</v>
+      </c>
+      <c r="D94" t="s">
+        <v>2</v>
+      </c>
+      <c r="E94">
+        <v>1</v>
+      </c>
+      <c r="F94" t="s">
+        <v>3</v>
+      </c>
+      <c r="G94">
+        <v>1</v>
+      </c>
+      <c r="H94" t="s">
+        <v>4</v>
+      </c>
+      <c r="I94">
+        <v>50</v>
+      </c>
+      <c r="K94">
+        <f>AVERAGE($G$1:G94)</f>
+        <v>-0.1276595744680851</v>
+      </c>
+      <c r="L94">
+        <f>AVERAGE($E$1:E94)</f>
+        <v>0.43617021276595747</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
+        <v>0</v>
+      </c>
+      <c r="C95" t="s">
+        <v>1</v>
+      </c>
+      <c r="D95" t="s">
+        <v>2</v>
+      </c>
+      <c r="E95">
+        <v>1</v>
+      </c>
+      <c r="F95" t="s">
+        <v>3</v>
+      </c>
+      <c r="G95">
+        <v>1</v>
+      </c>
+      <c r="H95" t="s">
+        <v>4</v>
+      </c>
+      <c r="I95">
+        <v>51</v>
+      </c>
+      <c r="K95">
+        <f>AVERAGE($G$1:G95)</f>
+        <v>-0.11578947368421053</v>
+      </c>
+      <c r="L95">
+        <f>AVERAGE($E$1:E95)</f>
+        <v>0.44210526315789472</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>0</v>
+      </c>
+      <c r="C96" t="s">
+        <v>1</v>
+      </c>
+      <c r="D96" t="s">
+        <v>2</v>
+      </c>
+      <c r="E96">
+        <v>1</v>
+      </c>
+      <c r="F96" t="s">
+        <v>3</v>
+      </c>
+      <c r="G96">
+        <v>1</v>
+      </c>
+      <c r="H96" t="s">
+        <v>4</v>
+      </c>
+      <c r="I96">
+        <v>54</v>
+      </c>
+      <c r="K96">
+        <f>AVERAGE($G$1:G96)</f>
+        <v>-0.10416666666666667</v>
+      </c>
+      <c r="L96">
+        <f>AVERAGE($E$1:E96)</f>
+        <v>0.44791666666666669</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>0</v>
+      </c>
+      <c r="C97" t="s">
+        <v>1</v>
+      </c>
+      <c r="D97" t="s">
+        <v>2</v>
+      </c>
+      <c r="E97">
+        <v>1</v>
+      </c>
+      <c r="F97" t="s">
+        <v>3</v>
+      </c>
+      <c r="G97">
+        <v>1</v>
+      </c>
+      <c r="H97" t="s">
+        <v>4</v>
+      </c>
+      <c r="I97">
+        <v>49</v>
+      </c>
+      <c r="K97">
+        <f>AVERAGE($G$1:G97)</f>
+        <v>-9.2783505154639179E-2</v>
+      </c>
+      <c r="L97">
+        <f>AVERAGE($E$1:E97)</f>
+        <v>0.45360824742268041</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>0</v>
+      </c>
+      <c r="C98" t="s">
+        <v>1</v>
+      </c>
+      <c r="D98" t="s">
+        <v>2</v>
+      </c>
+      <c r="E98">
+        <v>1</v>
+      </c>
+      <c r="F98" t="s">
+        <v>3</v>
+      </c>
+      <c r="G98">
+        <v>1</v>
+      </c>
+      <c r="H98" t="s">
+        <v>4</v>
+      </c>
+      <c r="I98">
+        <v>50</v>
+      </c>
+      <c r="K98">
+        <f>AVERAGE($G$1:G98)</f>
+        <v>-8.1632653061224483E-2</v>
+      </c>
+      <c r="L98">
+        <f>AVERAGE($E$1:E98)</f>
+        <v>0.45918367346938777</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>0</v>
+      </c>
+      <c r="C99" t="s">
+        <v>1</v>
+      </c>
+      <c r="D99" t="s">
+        <v>2</v>
+      </c>
+      <c r="E99">
+        <v>1</v>
+      </c>
+      <c r="F99" t="s">
+        <v>3</v>
+      </c>
+      <c r="G99">
+        <v>1</v>
+      </c>
+      <c r="H99" t="s">
+        <v>4</v>
+      </c>
+      <c r="I99">
+        <v>51</v>
+      </c>
+      <c r="K99">
+        <f>AVERAGE($G$1:G99)</f>
+        <v>-7.0707070707070704E-2</v>
+      </c>
+      <c r="L99">
+        <f>AVERAGE($E$1:E99)</f>
+        <v>0.46464646464646464</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>0</v>
+      </c>
+      <c r="C100" t="s">
+        <v>1</v>
+      </c>
+      <c r="D100" t="s">
+        <v>2</v>
+      </c>
+      <c r="E100">
+        <v>1</v>
+      </c>
+      <c r="F100" t="s">
+        <v>3</v>
+      </c>
+      <c r="G100">
+        <v>1</v>
+      </c>
+      <c r="H100" t="s">
+        <v>4</v>
+      </c>
+      <c r="I100">
+        <v>54</v>
+      </c>
+      <c r="K100">
+        <f>AVERAGE($G$1:G100)</f>
+        <v>-0.06</v>
+      </c>
+      <c r="L100">
+        <f>AVERAGE($E$1:E100)</f>
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12">
+      <c r="B101" t="s">
+        <v>0</v>
+      </c>
+      <c r="C101" t="s">
+        <v>1</v>
+      </c>
+      <c r="D101" t="s">
+        <v>2</v>
+      </c>
+      <c r="E101">
+        <v>1</v>
+      </c>
+      <c r="F101" t="s">
+        <v>3</v>
+      </c>
+      <c r="G101">
+        <v>1</v>
+      </c>
+      <c r="H101" t="s">
+        <v>4</v>
+      </c>
+      <c r="I101">
+        <v>47</v>
+      </c>
+      <c r="K101">
+        <f>AVERAGE($G$1:G101)</f>
+        <v>-4.9504950495049507E-2</v>
+      </c>
+      <c r="L101">
+        <f>AVERAGE($E$1:E101)</f>
+        <v>0.47524752475247523</v>
       </c>
     </row>
   </sheetData>

</xml_diff>